<commit_message>
finalize shipley OES lookup; continue evolution of generic method
</commit_message>
<xml_diff>
--- a/INPUT-FILES/SHIPLEY/CV68.xlsx
+++ b/INPUT-FILES/SHIPLEY/CV68.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eklaassen\Desktop\Misc\Shipley norms task\For Dave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC6BCB-C095-4A98-836A-447DF3E4E412}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A53A74-FE27-42D0-98D3-24F79B60D55A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adult" sheetId="1" r:id="rId1"/>
+    <sheet name="child" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="500" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>agestrat</t>
   </si>
@@ -51,6 +52,12 @@
   </si>
   <si>
     <t>CMB_CV68</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>096</t>
   </si>
 </sst>
 </file>
@@ -86,8 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,4 +575,225 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E845ED0D-915D-42DA-ABAE-8AACDBFB11FB}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>132</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>144</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>156</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>180</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>204</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>